<commit_message>
Remove oneway-specific bike lane LTS
</commit_message>
<xml_diff>
--- a/pybna/sql/stress/tables/stress_bike_lane.xlsx
+++ b/pybna/sql/stress/tables/stress_bike_lane.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\pybna\pybna\sql\stress\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53AFC549-5828-430B-A42D-2581DC41C4C3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E554D084-13F9-4934-89FE-DDA6A46FADE6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F31A81E7-F0F4-47CF-B45A-C4DA9B9EE623}"/>
+    <workbookView xWindow="30255" yWindow="2745" windowWidth="21600" windowHeight="11775" xr2:uid="{F31A81E7-F0F4-47CF-B45A-C4DA9B9EE623}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="9">
   <si>
     <t>f</t>
   </si>
@@ -409,11 +409,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B444F16D-22D4-4BD5-8243-27F9ED583C8A}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L56" sqref="L56"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1685,9 +1685,6 @@
       <c r="A64">
         <v>3</v>
       </c>
-      <c r="B64" t="s">
-        <v>1</v>
-      </c>
       <c r="C64" t="s">
         <v>1</v>
       </c>
@@ -1695,22 +1692,19 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F64">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G64">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>3</v>
       </c>
-      <c r="B65" t="s">
-        <v>1</v>
-      </c>
       <c r="C65" t="s">
         <v>1</v>
       </c>
@@ -1718,21 +1712,18 @@
         <v>0</v>
       </c>
       <c r="E65">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F65">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="G65">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>3</v>
-      </c>
-      <c r="B66" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C66" t="s">
         <v>1</v>
@@ -1741,10 +1732,10 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F66">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G66">
         <v>3</v>
@@ -1752,10 +1743,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>3</v>
-      </c>
-      <c r="B67" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C67" t="s">
         <v>1</v>
@@ -1764,21 +1752,18 @@
         <v>0</v>
       </c>
       <c r="E67">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F67">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="G67">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>3</v>
-      </c>
-      <c r="B68" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C68" t="s">
         <v>1</v>
@@ -1787,18 +1772,18 @@
         <v>0</v>
       </c>
       <c r="E68">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F68">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="G68">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C69" t="s">
         <v>1</v>
@@ -1810,15 +1795,15 @@
         <v>4</v>
       </c>
       <c r="F69">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="G69">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
@@ -1830,15 +1815,15 @@
         <v>4</v>
       </c>
       <c r="F70">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="G70">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
@@ -1850,109 +1835,9 @@
         <v>4</v>
       </c>
       <c r="F71">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="G71">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>4</v>
-      </c>
-      <c r="C72" t="s">
-        <v>1</v>
-      </c>
-      <c r="D72" t="s">
-        <v>0</v>
-      </c>
-      <c r="E72">
-        <v>4</v>
-      </c>
-      <c r="F72">
-        <v>99</v>
-      </c>
-      <c r="G72">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>5</v>
-      </c>
-      <c r="C73" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" t="s">
-        <v>0</v>
-      </c>
-      <c r="E73">
-        <v>4</v>
-      </c>
-      <c r="F73">
-        <v>40</v>
-      </c>
-      <c r="G73">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>5</v>
-      </c>
-      <c r="C74" t="s">
-        <v>1</v>
-      </c>
-      <c r="D74" t="s">
-        <v>0</v>
-      </c>
-      <c r="E74">
-        <v>4</v>
-      </c>
-      <c r="F74">
-        <v>99</v>
-      </c>
-      <c r="G74">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>6</v>
-      </c>
-      <c r="C75" t="s">
-        <v>1</v>
-      </c>
-      <c r="D75" t="s">
-        <v>0</v>
-      </c>
-      <c r="E75">
-        <v>4</v>
-      </c>
-      <c r="F75">
-        <v>40</v>
-      </c>
-      <c r="G75">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>6</v>
-      </c>
-      <c r="C76" t="s">
-        <v>1</v>
-      </c>
-      <c r="D76" t="s">
-        <v>0</v>
-      </c>
-      <c r="E76">
-        <v>4</v>
-      </c>
-      <c r="F76">
-        <v>99</v>
-      </c>
-      <c r="G76">
         <v>4</v>
       </c>
     </row>

</xml_diff>